<commit_message>
Version 1.4 Output Excel file has students organized in columns based on their subject group
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -424,29 +424,29 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>K1</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>F2</t>
+          <t>F3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>K2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -456,13 +456,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>F3</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>F2</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>